<commit_message>
exemplo xlsx rstac; ajuste faq
</commit_message>
<xml_diff>
--- a/flask/app/static/examples/CC_DIMCI_0496_2025.xlsx
+++ b/flask/app/static/examples/CC_DIMCI_0496_2025.xlsx
@@ -5,20 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadados Principais" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Software" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Cliente" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Informações Pertinentes" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="Declarações" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Rastreabilidade" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Método de Medição" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="Mensurando" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="Índices" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="Resultados" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="Observações" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="Metadados Principais" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Software" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Cliente" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Informações Pertinentes" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Declarações" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Rastreabilidade" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Método de Medição" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Mensurando" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Índices" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Resultados" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Observações" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t xml:space="preserve">Campo</t>
   </si>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">refType</t>
   </si>
   <si>
-    <t xml:space="preserve">Temperatura</t>
+    <t xml:space="preserve">Temperatura no banho de ar</t>
   </si>
   <si>
     <t xml:space="preserve">\degreecelsius</t>
@@ -278,10 +278,7 @@
     <t xml:space="preserve">DIMCI 1263/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">PR 465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equation</t>
+    <t xml:space="preserve">Lampe PR 465</t>
   </si>
   <si>
     <t xml:space="preserve">O resultado fornecido refere-se ao valor médio de três séries de seis medições pelo método de comparação potenciométrico por divisor de tensão binário na configuração de 04 (quatro) terminais. Utilizou-se uma ponte automática de resistência modelo 6000A.</t>
@@ -444,178 +441,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office">
-  <a:themeElements>
-    <a:clrScheme name="Escritório">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Escritório">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -623,13 +448,13 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="62.42"/>
@@ -893,7 +718,7 @@
       <selection pane="bottomLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
@@ -906,10 +731,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>62</v>
@@ -923,7 +748,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10</v>
@@ -962,14 +787,14 @@
       <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -990,13 +815,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.2"/>
@@ -1043,7 +868,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.57"/>
@@ -1131,10 +956,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.42"/>
@@ -1189,7 +1014,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>54.5</v>
+        <v>54.4</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2.8</v>
@@ -1225,7 +1050,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="242.42"/>
@@ -1276,10 +1101,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.57"/>
@@ -1336,10 +1161,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="118.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.14"/>
@@ -1349,13 +1174,11 @@
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1382,7 +1205,7 @@
       <selection pane="bottomLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.71"/>
@@ -1394,19 +1217,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>67</v>
@@ -1414,16 +1237,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>33</v>
@@ -1453,7 +1276,7 @@
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="14.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.57"/>
@@ -1461,10 +1284,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>42</v>
@@ -1478,16 +1301,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>